<commit_message>
Format all source codes
</commit_message>
<xml_diff>
--- a/user_input/ngung_giao_nhan.xlsx
+++ b/user_input/ngung_giao_nhan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\QLRR\Cập nhật quá tải\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EFA6C7-D535-4230-B306-F2FD4996A31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2094BB42-91FD-4177-AD73-CBC428450C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2305" uniqueCount="1444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2228" uniqueCount="1444">
   <si>
     <t>TT</t>
   </si>
@@ -4783,8 +4783,8 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5108,7 +5108,9 @@
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
+      <c r="I12" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
@@ -5262,9 +5264,7 @@
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
-      <c r="I18" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="I18" s="10"/>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
@@ -5339,13 +5339,9 @@
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
-      <c r="I21" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="I21" s="10"/>
       <c r="J21" s="10"/>
-      <c r="K21" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="K21" s="10"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
     </row>
@@ -5442,9 +5438,7 @@
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
-      <c r="H25" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="H25" s="10"/>
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -5545,9 +5539,7 @@
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
-      <c r="I29" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="I29" s="10"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
@@ -6247,9 +6239,7 @@
         <v>21</v>
       </c>
       <c r="F57" s="10"/>
-      <c r="G57" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G57" s="10"/>
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
       <c r="J57" s="10"/>
@@ -6305,7 +6295,9 @@
       <c r="J59" s="10"/>
       <c r="K59" s="10"/>
       <c r="L59" s="10"/>
-      <c r="M59" s="10"/>
+      <c r="M59" s="10" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="60" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="10">
@@ -6399,13 +6391,11 @@
         <v>141</v>
       </c>
       <c r="F63" s="10"/>
-      <c r="G63" s="10" t="s">
+      <c r="G63" s="10"/>
+      <c r="H63" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="H63" s="10"/>
-      <c r="I63" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="I63" s="10"/>
       <c r="J63" s="10"/>
       <c r="K63" s="10"/>
       <c r="L63" s="10"/>
@@ -6428,9 +6418,13 @@
         <v>143</v>
       </c>
       <c r="F64" s="10"/>
-      <c r="G64" s="10"/>
+      <c r="G64" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="H64" s="10"/>
-      <c r="I64" s="10"/>
+      <c r="I64" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="J64" s="10"/>
       <c r="K64" s="10"/>
       <c r="L64" s="10"/>
@@ -6459,9 +6453,7 @@
       <c r="H65" s="10"/>
       <c r="I65" s="10"/>
       <c r="J65" s="10"/>
-      <c r="K65" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="K65" s="10"/>
       <c r="L65" s="10"/>
       <c r="M65" s="10"/>
     </row>
@@ -6511,9 +6503,7 @@
         <v>43</v>
       </c>
       <c r="H67" s="10"/>
-      <c r="I67" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="I67" s="10"/>
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
       <c r="L67" s="10"/>
@@ -6538,9 +6528,7 @@
       <c r="F68" s="10"/>
       <c r="G68" s="10"/>
       <c r="H68" s="10"/>
-      <c r="I68" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="I68" s="10"/>
       <c r="J68" s="10"/>
       <c r="K68" s="10"/>
       <c r="L68" s="10"/>
@@ -6562,18 +6550,18 @@
       <c r="E69" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="F69" s="10"/>
+      <c r="F69" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="G69" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="H69" s="10"/>
-      <c r="I69" s="10" t="s">
+      <c r="H69" s="10" t="s">
         <v>43</v>
       </c>
+      <c r="I69" s="10"/>
       <c r="J69" s="10"/>
-      <c r="K69" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="K69" s="10"/>
       <c r="L69" s="10"/>
       <c r="M69" s="10"/>
     </row>
@@ -6598,9 +6586,7 @@
         <v>43</v>
       </c>
       <c r="H70" s="10"/>
-      <c r="I70" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="I70" s="10"/>
       <c r="J70" s="10"/>
       <c r="K70" s="10"/>
       <c r="L70" s="10"/>
@@ -6627,7 +6613,9 @@
         <v>43</v>
       </c>
       <c r="H71" s="10"/>
-      <c r="I71" s="10"/>
+      <c r="I71" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="J71" s="10"/>
       <c r="K71" s="10"/>
       <c r="L71" s="10"/>
@@ -6750,9 +6738,7 @@
         <v>168</v>
       </c>
       <c r="F76" s="10"/>
-      <c r="G76" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G76" s="10"/>
       <c r="H76" s="10"/>
       <c r="I76" s="10"/>
       <c r="J76" s="10"/>
@@ -6953,12 +6939,12 @@
       </c>
       <c r="F84" s="10"/>
       <c r="G84" s="10"/>
-      <c r="H84" s="10"/>
+      <c r="H84" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="I84" s="10"/>
       <c r="J84" s="10"/>
-      <c r="K84" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="K84" s="10"/>
       <c r="L84" s="10"/>
       <c r="M84" s="10"/>
     </row>
@@ -6980,7 +6966,9 @@
       </c>
       <c r="F85" s="10"/>
       <c r="G85" s="10"/>
-      <c r="H85" s="10"/>
+      <c r="H85" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="I85" s="10"/>
       <c r="J85" s="10"/>
       <c r="K85" s="10"/>
@@ -7080,7 +7068,9 @@
       </c>
       <c r="F89" s="10"/>
       <c r="G89" s="10"/>
-      <c r="H89" s="10"/>
+      <c r="H89" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="I89" s="10"/>
       <c r="J89" s="10"/>
       <c r="K89" s="10"/>
@@ -7180,7 +7170,9 @@
       </c>
       <c r="F93" s="10"/>
       <c r="G93" s="10"/>
-      <c r="H93" s="10"/>
+      <c r="H93" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="I93" s="10"/>
       <c r="J93" s="10"/>
       <c r="K93" s="10"/>
@@ -7479,9 +7471,7 @@
         <v>228</v>
       </c>
       <c r="F105" s="10"/>
-      <c r="G105" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G105" s="10"/>
       <c r="H105" s="10"/>
       <c r="I105" s="10"/>
       <c r="J105" s="10"/>
@@ -8232,9 +8222,7 @@
       </c>
       <c r="F135" s="10"/>
       <c r="G135" s="10"/>
-      <c r="H135" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="H135" s="10"/>
       <c r="I135" s="10"/>
       <c r="J135" s="10"/>
       <c r="K135" s="10"/>
@@ -8284,9 +8272,7 @@
       </c>
       <c r="F137" s="10"/>
       <c r="G137" s="10"/>
-      <c r="H137" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="H137" s="10"/>
       <c r="I137" s="10"/>
       <c r="J137" s="10"/>
       <c r="K137" s="10"/>
@@ -8411,14 +8397,10 @@
       </c>
       <c r="F142" s="10"/>
       <c r="G142" s="10"/>
-      <c r="H142" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="H142" s="10"/>
       <c r="I142" s="10"/>
       <c r="J142" s="10"/>
-      <c r="K142" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="K142" s="10"/>
       <c r="L142" s="10"/>
       <c r="M142" s="10"/>
     </row>
@@ -8489,12 +8471,8 @@
         <v>308</v>
       </c>
       <c r="F145" s="10"/>
-      <c r="G145" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H145" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G145" s="10"/>
+      <c r="H145" s="10"/>
       <c r="I145" s="10"/>
       <c r="J145" s="10"/>
       <c r="K145" s="10"/>
@@ -8593,9 +8571,7 @@
         <v>316</v>
       </c>
       <c r="F149" s="10"/>
-      <c r="G149" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G149" s="10"/>
       <c r="H149" s="10"/>
       <c r="I149" s="10"/>
       <c r="J149" s="10"/>
@@ -8695,9 +8671,7 @@
         <v>324</v>
       </c>
       <c r="F153" s="10"/>
-      <c r="G153" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G153" s="10"/>
       <c r="H153" s="10"/>
       <c r="I153" s="10"/>
       <c r="J153" s="10"/>
@@ -8722,9 +8696,7 @@
         <v>326</v>
       </c>
       <c r="F154" s="10"/>
-      <c r="G154" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G154" s="10"/>
       <c r="H154" s="10"/>
       <c r="I154" s="10"/>
       <c r="J154" s="10"/>
@@ -8749,9 +8721,7 @@
         <v>328</v>
       </c>
       <c r="F155" s="10"/>
-      <c r="G155" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G155" s="10"/>
       <c r="H155" s="10"/>
       <c r="I155" s="10"/>
       <c r="J155" s="10"/>
@@ -8926,7 +8896,9 @@
         <v>343</v>
       </c>
       <c r="F162" s="10"/>
-      <c r="G162" s="10"/>
+      <c r="G162" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="H162" s="10"/>
       <c r="I162" s="10"/>
       <c r="J162" s="10"/>
@@ -8951,7 +8923,9 @@
         <v>345</v>
       </c>
       <c r="F163" s="10"/>
-      <c r="G163" s="10"/>
+      <c r="G163" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="H163" s="10"/>
       <c r="I163" s="10"/>
       <c r="J163" s="10"/>
@@ -8975,9 +8949,7 @@
       <c r="E164" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="F164" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="F164" s="10"/>
       <c r="G164" s="10"/>
       <c r="H164" s="10"/>
       <c r="I164" s="10"/>
@@ -9003,7 +8975,9 @@
         <v>349</v>
       </c>
       <c r="F165" s="10"/>
-      <c r="G165" s="10"/>
+      <c r="G165" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="H165" s="10"/>
       <c r="I165" s="10"/>
       <c r="J165" s="10"/>
@@ -9028,9 +9002,7 @@
         <v>352</v>
       </c>
       <c r="F166" s="10"/>
-      <c r="G166" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G166" s="10"/>
       <c r="H166" s="10"/>
       <c r="I166" s="10"/>
       <c r="J166" s="10"/>
@@ -9282,9 +9254,7 @@
       <c r="F176" s="10"/>
       <c r="G176" s="10"/>
       <c r="H176" s="10"/>
-      <c r="I176" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="I176" s="10"/>
       <c r="J176" s="10"/>
       <c r="K176" s="10"/>
       <c r="L176" s="10"/>
@@ -9308,9 +9278,7 @@
       </c>
       <c r="F177" s="10"/>
       <c r="G177" s="10"/>
-      <c r="H177" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="H177" s="10"/>
       <c r="I177" s="10"/>
       <c r="J177" s="10"/>
       <c r="K177" s="10"/>
@@ -9540,7 +9508,9 @@
       </c>
       <c r="I186" s="10"/>
       <c r="J186" s="10"/>
-      <c r="K186" s="10"/>
+      <c r="K186" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="L186" s="10"/>
       <c r="M186" s="10"/>
     </row>
@@ -10010,9 +9980,7 @@
       <c r="E205" s="11" t="s">
         <v>429</v>
       </c>
-      <c r="F205" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="F205" s="10"/>
       <c r="G205" s="10"/>
       <c r="H205" s="10"/>
       <c r="I205" s="10"/>
@@ -10362,7 +10330,9 @@
       <c r="E219" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="F219" s="10"/>
+      <c r="F219" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="G219" s="10"/>
       <c r="H219" s="10"/>
       <c r="I219" s="10"/>
@@ -10790,10 +10760,10 @@
         <v>494</v>
       </c>
       <c r="F236" s="10"/>
-      <c r="G236" s="10"/>
-      <c r="H236" s="10" t="s">
+      <c r="G236" s="10" t="s">
         <v>43</v>
       </c>
+      <c r="H236" s="10"/>
       <c r="I236" s="10"/>
       <c r="J236" s="10"/>
       <c r="K236" s="10"/>
@@ -10818,9 +10788,7 @@
       </c>
       <c r="F237" s="10"/>
       <c r="G237" s="10"/>
-      <c r="H237" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="H237" s="10"/>
       <c r="I237" s="10"/>
       <c r="J237" s="10"/>
       <c r="K237" s="10"/>
@@ -10869,7 +10837,9 @@
         <v>500</v>
       </c>
       <c r="F239" s="10"/>
-      <c r="G239" s="10"/>
+      <c r="G239" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="H239" s="10" t="s">
         <v>43</v>
       </c>
@@ -10896,7 +10866,9 @@
         <v>502</v>
       </c>
       <c r="F240" s="10"/>
-      <c r="G240" s="10"/>
+      <c r="G240" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="H240" s="10" t="s">
         <v>43</v>
       </c>
@@ -11076,9 +11048,7 @@
       </c>
       <c r="F247" s="10"/>
       <c r="G247" s="10"/>
-      <c r="H247" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="H247" s="10"/>
       <c r="I247" s="10"/>
       <c r="J247" s="10"/>
       <c r="K247" s="10"/>
@@ -11305,9 +11275,7 @@
       </c>
       <c r="F256" s="10"/>
       <c r="G256" s="10"/>
-      <c r="H256" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="H256" s="10"/>
       <c r="I256" s="10"/>
       <c r="J256" s="10"/>
       <c r="K256" s="10"/>
@@ -11382,7 +11350,9 @@
       </c>
       <c r="F259" s="10"/>
       <c r="G259" s="10"/>
-      <c r="H259" s="10"/>
+      <c r="H259" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="I259" s="10"/>
       <c r="J259" s="10"/>
       <c r="K259" s="10"/>
@@ -11407,9 +11377,7 @@
       </c>
       <c r="F260" s="10"/>
       <c r="G260" s="10"/>
-      <c r="H260" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="H260" s="10"/>
       <c r="I260" s="10"/>
       <c r="J260" s="10"/>
       <c r="K260" s="10"/>
@@ -11757,7 +11725,9 @@
       <c r="E274" s="11" t="s">
         <v>570</v>
       </c>
-      <c r="F274" s="10"/>
+      <c r="F274" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="G274" s="10"/>
       <c r="H274" s="10"/>
       <c r="I274" s="10"/>
@@ -11833,9 +11803,7 @@
         <v>577</v>
       </c>
       <c r="F277" s="10"/>
-      <c r="G277" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G277" s="10"/>
       <c r="H277" s="10"/>
       <c r="I277" s="10"/>
       <c r="J277" s="10"/>
@@ -11860,9 +11828,7 @@
         <v>579</v>
       </c>
       <c r="F278" s="10"/>
-      <c r="G278" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G278" s="10"/>
       <c r="H278" s="10"/>
       <c r="I278" s="10"/>
       <c r="J278" s="10"/>
@@ -11912,9 +11878,7 @@
         <v>583</v>
       </c>
       <c r="F280" s="10"/>
-      <c r="G280" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G280" s="10"/>
       <c r="H280" s="10"/>
       <c r="I280" s="10"/>
       <c r="J280" s="10"/>
@@ -11989,7 +11953,9 @@
         <v>589</v>
       </c>
       <c r="F283" s="10"/>
-      <c r="G283" s="10"/>
+      <c r="G283" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="H283" s="10"/>
       <c r="I283" s="10"/>
       <c r="J283" s="10"/>
@@ -12039,7 +12005,9 @@
         <v>593</v>
       </c>
       <c r="F285" s="10"/>
-      <c r="G285" s="10"/>
+      <c r="G285" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="H285" s="10"/>
       <c r="I285" s="10"/>
       <c r="J285" s="10"/>
@@ -12243,9 +12211,7 @@
         <v>608</v>
       </c>
       <c r="F293" s="10"/>
-      <c r="G293" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G293" s="10"/>
       <c r="H293" s="10"/>
       <c r="I293" s="10"/>
       <c r="J293" s="10"/>
@@ -12270,7 +12236,9 @@
         <v>610</v>
       </c>
       <c r="F294" s="10"/>
-      <c r="G294" s="10"/>
+      <c r="G294" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="H294" s="10"/>
       <c r="I294" s="10"/>
       <c r="J294" s="10"/>
@@ -12370,9 +12338,7 @@
         <v>618</v>
       </c>
       <c r="F298" s="10"/>
-      <c r="G298" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G298" s="10"/>
       <c r="H298" s="10"/>
       <c r="I298" s="10"/>
       <c r="J298" s="10"/>
@@ -12697,13 +12663,11 @@
         <v>643</v>
       </c>
       <c r="F311" s="10"/>
-      <c r="G311" s="10"/>
-      <c r="H311" s="10" t="s">
+      <c r="G311" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I311" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="H311" s="10"/>
+      <c r="I311" s="10"/>
       <c r="J311" s="10"/>
       <c r="K311" s="10"/>
       <c r="L311" s="10"/>
@@ -12729,9 +12693,7 @@
       <c r="G312" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="H312" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="H312" s="10"/>
       <c r="I312" s="10"/>
       <c r="J312" s="10"/>
       <c r="K312" s="10"/>
@@ -12858,9 +12820,7 @@
       </c>
       <c r="F317" s="10"/>
       <c r="G317" s="10"/>
-      <c r="H317" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="H317" s="10"/>
       <c r="I317" s="10"/>
       <c r="J317" s="10"/>
       <c r="K317" s="10"/>
@@ -12883,9 +12843,7 @@
       <c r="E318" s="11" t="s">
         <v>657</v>
       </c>
-      <c r="F318" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="F318" s="10"/>
       <c r="G318" s="10"/>
       <c r="H318" s="10"/>
       <c r="I318" s="10"/>
@@ -12911,9 +12869,7 @@
         <v>659</v>
       </c>
       <c r="F319" s="10"/>
-      <c r="G319" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G319" s="10"/>
       <c r="H319" s="10"/>
       <c r="I319" s="10"/>
       <c r="J319" s="10"/>
@@ -12990,9 +12946,7 @@
         <v>662</v>
       </c>
       <c r="F322" s="10"/>
-      <c r="G322" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G322" s="10"/>
       <c r="H322" s="10"/>
       <c r="I322" s="10"/>
       <c r="J322" s="10"/>
@@ -13017,12 +12971,8 @@
         <v>663</v>
       </c>
       <c r="F323" s="10"/>
-      <c r="G323" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H323" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G323" s="10"/>
+      <c r="H323" s="10"/>
       <c r="I323" s="10"/>
       <c r="J323" s="10"/>
       <c r="K323" s="10"/>
@@ -13229,9 +13179,7 @@
       <c r="H331" s="10"/>
       <c r="I331" s="10"/>
       <c r="J331" s="10"/>
-      <c r="K331" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="K331" s="10"/>
       <c r="L331" s="10"/>
       <c r="M331" s="10"/>
     </row>
@@ -13253,9 +13201,7 @@
       </c>
       <c r="F332" s="10"/>
       <c r="G332" s="10"/>
-      <c r="H332" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="H332" s="10"/>
       <c r="I332" s="10"/>
       <c r="J332" s="10"/>
       <c r="K332" s="10"/>
@@ -13304,12 +13250,8 @@
         <v>676</v>
       </c>
       <c r="F334" s="10"/>
-      <c r="G334" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H334" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G334" s="10"/>
+      <c r="H334" s="10"/>
       <c r="I334" s="10"/>
       <c r="J334" s="10"/>
       <c r="K334" s="10"/>
@@ -13359,9 +13301,7 @@
       </c>
       <c r="F336" s="10"/>
       <c r="G336" s="10"/>
-      <c r="H336" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="H336" s="10"/>
       <c r="I336" s="10"/>
       <c r="J336" s="10"/>
       <c r="K336" s="10"/>
@@ -13711,9 +13651,7 @@
       </c>
       <c r="F350" s="10"/>
       <c r="G350" s="10"/>
-      <c r="H350" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="H350" s="10"/>
       <c r="I350" s="10"/>
       <c r="J350" s="10"/>
       <c r="K350" s="10"/>
@@ -13887,9 +13825,7 @@
         <v>725</v>
       </c>
       <c r="F357" s="10"/>
-      <c r="G357" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G357" s="10"/>
       <c r="H357" s="10"/>
       <c r="I357" s="10"/>
       <c r="J357" s="10"/>
@@ -13914,9 +13850,7 @@
         <v>727</v>
       </c>
       <c r="F358" s="10"/>
-      <c r="G358" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G358" s="10"/>
       <c r="H358" s="10"/>
       <c r="I358" s="10"/>
       <c r="J358" s="10"/>
@@ -13991,9 +13925,7 @@
         <v>733</v>
       </c>
       <c r="F361" s="10"/>
-      <c r="G361" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G361" s="10"/>
       <c r="H361" s="10"/>
       <c r="I361" s="10"/>
       <c r="J361" s="10"/>
@@ -14042,12 +13974,8 @@
       <c r="E363" s="11" t="s">
         <v>737</v>
       </c>
-      <c r="F363" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G363" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="F363" s="10"/>
+      <c r="G363" s="10"/>
       <c r="H363" s="10"/>
       <c r="I363" s="10"/>
       <c r="J363" s="10"/>
@@ -14305,9 +14233,7 @@
       <c r="H373" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I373" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="I373" s="10"/>
       <c r="J373" s="10"/>
       <c r="K373" s="10"/>
       <c r="L373" s="10"/>
@@ -14361,9 +14287,7 @@
       <c r="H375" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I375" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="I375" s="10"/>
       <c r="J375" s="10"/>
       <c r="K375" s="10"/>
       <c r="L375" s="10"/>
@@ -14839,7 +14763,9 @@
       </c>
       <c r="F394" s="10"/>
       <c r="G394" s="10"/>
-      <c r="H394" s="10"/>
+      <c r="H394" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="I394" s="10"/>
       <c r="J394" s="10"/>
       <c r="K394" s="10"/>
@@ -14937,7 +14863,9 @@
       <c r="E398" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="F398" s="10"/>
+      <c r="F398" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="G398" s="10"/>
       <c r="H398" s="10"/>
       <c r="I398" s="10"/>
@@ -15019,7 +14947,9 @@
       <c r="H401" s="10"/>
       <c r="I401" s="10"/>
       <c r="J401" s="10"/>
-      <c r="K401" s="10"/>
+      <c r="K401" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="L401" s="10"/>
       <c r="M401" s="10"/>
     </row>
@@ -15069,9 +14999,7 @@
         <v>43</v>
       </c>
       <c r="H403" s="10"/>
-      <c r="I403" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="I403" s="10"/>
       <c r="J403" s="10"/>
       <c r="K403" s="10"/>
       <c r="L403" s="10"/>
@@ -15119,7 +15047,9 @@
         <v>820</v>
       </c>
       <c r="F405" s="10"/>
-      <c r="G405" s="10"/>
+      <c r="G405" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="H405" s="10"/>
       <c r="I405" s="10"/>
       <c r="J405" s="10"/>
@@ -15144,10 +15074,7 @@
         <v>822</v>
       </c>
       <c r="F406" s="10"/>
-      <c r="G406" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H406" s="10"/>
+      <c r="G406" s="10"/>
       <c r="I406" s="10"/>
       <c r="J406" s="10"/>
       <c r="K406" s="10"/>
@@ -15376,9 +15303,7 @@
       </c>
       <c r="F415" s="10"/>
       <c r="G415" s="10"/>
-      <c r="H415" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="H415" s="10"/>
       <c r="I415" s="10"/>
       <c r="J415" s="10"/>
       <c r="K415" s="10"/>
@@ -15552,9 +15477,7 @@
         <v>856</v>
       </c>
       <c r="F422" s="10"/>
-      <c r="G422" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G422" s="10"/>
       <c r="H422" s="10"/>
       <c r="I422" s="10"/>
       <c r="J422" s="10"/>
@@ -15629,9 +15552,7 @@
         <v>862</v>
       </c>
       <c r="F425" s="10"/>
-      <c r="G425" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G425" s="10"/>
       <c r="H425" s="10"/>
       <c r="I425" s="10"/>
       <c r="J425" s="10"/>
@@ -15856,12 +15777,8 @@
         <v>879</v>
       </c>
       <c r="F434" s="10"/>
-      <c r="G434" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H434" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G434" s="10"/>
+      <c r="H434" s="10"/>
       <c r="I434" s="10"/>
       <c r="J434" s="10"/>
       <c r="K434" s="10"/>
@@ -16435,12 +16352,8 @@
         <v>927</v>
       </c>
       <c r="F457" s="10"/>
-      <c r="G457" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H457" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G457" s="10"/>
+      <c r="H457" s="10"/>
       <c r="I457" s="10"/>
       <c r="J457" s="10"/>
       <c r="K457" s="10"/>
@@ -16465,7 +16378,9 @@
       </c>
       <c r="F458" s="10"/>
       <c r="G458" s="10"/>
-      <c r="H458" s="10"/>
+      <c r="H458" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="I458" s="10"/>
       <c r="J458" s="10"/>
       <c r="K458" s="10"/>
@@ -16567,7 +16482,9 @@
         <v>43</v>
       </c>
       <c r="G462" s="10"/>
-      <c r="H462" s="10"/>
+      <c r="H462" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="I462" s="10"/>
       <c r="J462" s="10"/>
       <c r="K462" s="10"/>
@@ -16790,11 +16707,11 @@
       <c r="E471" s="11" t="s">
         <v>952</v>
       </c>
-      <c r="F471" s="10" t="s">
+      <c r="F471" s="10"/>
+      <c r="G471" s="10"/>
+      <c r="H471" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G471" s="10"/>
-      <c r="H471" s="10"/>
       <c r="I471" s="10"/>
       <c r="J471" s="10"/>
       <c r="K471" s="10"/>
@@ -16822,7 +16739,9 @@
       <c r="H472" s="10"/>
       <c r="I472" s="10"/>
       <c r="J472" s="10"/>
-      <c r="K472" s="10"/>
+      <c r="K472" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="L472" s="10"/>
       <c r="M472" s="10"/>
     </row>
@@ -16867,9 +16786,7 @@
       <c r="E474" s="11" t="s">
         <v>958</v>
       </c>
-      <c r="F474" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="F474" s="10"/>
       <c r="G474" s="10"/>
       <c r="H474" s="10"/>
       <c r="I474" s="10"/>
@@ -17021,7 +16938,9 @@
       </c>
       <c r="F480" s="10"/>
       <c r="G480" s="10"/>
-      <c r="H480" s="10"/>
+      <c r="H480" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="I480" s="10"/>
       <c r="J480" s="10"/>
       <c r="K480" s="10"/>
@@ -17445,9 +17364,7 @@
         <v>408</v>
       </c>
       <c r="F497" s="10"/>
-      <c r="G497" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G497" s="10"/>
       <c r="H497" s="10"/>
       <c r="I497" s="10"/>
       <c r="J497" s="10"/>
@@ -17872,9 +17789,7 @@
         <v>1041</v>
       </c>
       <c r="F514" s="10"/>
-      <c r="G514" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G514" s="10"/>
       <c r="H514" s="10"/>
       <c r="I514" s="10"/>
       <c r="J514" s="10"/>
@@ -17899,9 +17814,7 @@
         <v>1043</v>
       </c>
       <c r="F515" s="10"/>
-      <c r="G515" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G515" s="10"/>
       <c r="H515" s="10"/>
       <c r="I515" s="10"/>
       <c r="J515" s="10"/>
@@ -18127,9 +18040,7 @@
       </c>
       <c r="F524" s="10"/>
       <c r="G524" s="10"/>
-      <c r="H524" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="H524" s="10"/>
       <c r="I524" s="10"/>
       <c r="J524" s="10"/>
       <c r="K524" s="10"/>
@@ -18177,9 +18088,7 @@
       <c r="E526" s="11" t="s">
         <v>1066</v>
       </c>
-      <c r="F526" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="F526" s="10"/>
       <c r="G526" s="10"/>
       <c r="H526" s="10"/>
       <c r="I526" s="10"/>
@@ -18205,9 +18114,7 @@
         <v>1068</v>
       </c>
       <c r="F527" s="10"/>
-      <c r="G527" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G527" s="10"/>
       <c r="H527" s="10"/>
       <c r="I527" s="10"/>
       <c r="J527" s="10"/>
@@ -18256,9 +18163,7 @@
       <c r="E529" s="11" t="s">
         <v>1072</v>
       </c>
-      <c r="F529" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="F529" s="10"/>
       <c r="G529" s="10"/>
       <c r="H529" s="10"/>
       <c r="I529" s="10"/>
@@ -18283,9 +18188,7 @@
       <c r="E530" s="11" t="s">
         <v>1074</v>
       </c>
-      <c r="F530" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="F530" s="10"/>
       <c r="G530" s="10"/>
       <c r="H530" s="10"/>
       <c r="I530" s="10"/>
@@ -18310,12 +18213,8 @@
       <c r="E531" s="11" t="s">
         <v>1076</v>
       </c>
-      <c r="F531" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G531" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="F531" s="10"/>
+      <c r="G531" s="10"/>
       <c r="H531" s="10"/>
       <c r="I531" s="10"/>
       <c r="J531" s="10"/>
@@ -18489,9 +18388,7 @@
       <c r="E538" s="11" t="s">
         <v>1090</v>
       </c>
-      <c r="F538" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="F538" s="10"/>
       <c r="G538" s="10"/>
       <c r="H538" s="10"/>
       <c r="I538" s="10"/>
@@ -18517,9 +18414,7 @@
         <v>1093</v>
       </c>
       <c r="F539" s="10"/>
-      <c r="G539" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G539" s="10"/>
       <c r="H539" s="10"/>
       <c r="I539" s="10"/>
       <c r="J539" s="10"/>
@@ -18544,9 +18439,7 @@
         <v>1095</v>
       </c>
       <c r="F540" s="10"/>
-      <c r="G540" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G540" s="10"/>
       <c r="H540" s="10"/>
       <c r="I540" s="10"/>
       <c r="J540" s="10"/>
@@ -18596,9 +18489,7 @@
         <v>1099</v>
       </c>
       <c r="F542" s="10"/>
-      <c r="G542" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G542" s="10"/>
       <c r="H542" s="10"/>
       <c r="I542" s="10"/>
       <c r="J542" s="10"/>
@@ -18698,9 +18589,7 @@
         <v>1107</v>
       </c>
       <c r="F546" s="10"/>
-      <c r="G546" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G546" s="10"/>
       <c r="H546" s="10"/>
       <c r="I546" s="10"/>
       <c r="J546" s="10"/>
@@ -18800,9 +18689,7 @@
         <v>1114</v>
       </c>
       <c r="F550" s="10"/>
-      <c r="G550" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G550" s="10"/>
       <c r="H550" s="10"/>
       <c r="I550" s="10"/>
       <c r="J550" s="10"/>
@@ -18827,9 +18714,7 @@
         <v>1116</v>
       </c>
       <c r="F551" s="10"/>
-      <c r="G551" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G551" s="10"/>
       <c r="H551" s="10"/>
       <c r="I551" s="10"/>
       <c r="J551" s="10"/>
@@ -19032,7 +18917,9 @@
       </c>
       <c r="F559" s="10"/>
       <c r="G559" s="10"/>
-      <c r="H559" s="10"/>
+      <c r="H559" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="I559" s="10"/>
       <c r="J559" s="10"/>
       <c r="K559" s="10"/>
@@ -19105,16 +18992,12 @@
       <c r="E562" s="11" t="s">
         <v>1139</v>
       </c>
-      <c r="F562" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="F562" s="10"/>
       <c r="G562" s="10"/>
       <c r="H562" s="10"/>
       <c r="I562" s="10"/>
       <c r="J562" s="10"/>
-      <c r="K562" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="K562" s="10"/>
       <c r="L562" s="10"/>
       <c r="M562" s="10"/>
     </row>
@@ -19760,9 +19643,7 @@
         <v>1192</v>
       </c>
       <c r="F588" s="10"/>
-      <c r="G588" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G588" s="10"/>
       <c r="H588" s="10"/>
       <c r="I588" s="10"/>
       <c r="J588" s="10"/>
@@ -19812,9 +19693,7 @@
         <v>1196</v>
       </c>
       <c r="F590" s="10"/>
-      <c r="G590" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G590" s="10"/>
       <c r="H590" s="10"/>
       <c r="I590" s="10"/>
       <c r="J590" s="10"/>
@@ -20264,13 +20143,9 @@
         <v>1230</v>
       </c>
       <c r="F608" s="10"/>
-      <c r="G608" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G608" s="10"/>
       <c r="H608" s="10"/>
-      <c r="I608" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="I608" s="10"/>
       <c r="J608" s="10"/>
       <c r="K608" s="10"/>
       <c r="L608" s="10"/>
@@ -20318,9 +20193,7 @@
         <v>1235</v>
       </c>
       <c r="F610" s="10"/>
-      <c r="G610" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G610" s="10"/>
       <c r="H610" s="10"/>
       <c r="I610" s="10"/>
       <c r="J610" s="10"/>
@@ -20395,10 +20268,10 @@
         <v>1241</v>
       </c>
       <c r="F613" s="10"/>
-      <c r="G613" s="10" t="s">
+      <c r="G613" s="10"/>
+      <c r="H613" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="H613" s="10"/>
       <c r="I613" s="10"/>
       <c r="J613" s="10"/>
       <c r="K613" s="10"/>
@@ -20422,7 +20295,9 @@
         <v>1243</v>
       </c>
       <c r="F614" s="10"/>
-      <c r="G614" s="10"/>
+      <c r="G614" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="H614" s="10"/>
       <c r="I614" s="10"/>
       <c r="J614" s="10"/>
@@ -20571,7 +20446,9 @@
       <c r="E620" s="11" t="s">
         <v>1256</v>
       </c>
-      <c r="F620" s="10"/>
+      <c r="F620" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="G620" s="13"/>
       <c r="H620" s="10"/>
       <c r="I620" s="10"/>
@@ -20848,7 +20725,9 @@
       </c>
       <c r="F631" s="10"/>
       <c r="G631" s="10"/>
-      <c r="H631" s="10"/>
+      <c r="H631" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="I631" s="10"/>
       <c r="J631" s="10"/>
       <c r="K631" s="10"/>
@@ -20972,9 +20851,7 @@
         <v>1289</v>
       </c>
       <c r="F636" s="10"/>
-      <c r="G636" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G636" s="10"/>
       <c r="H636" s="10"/>
       <c r="I636" s="10"/>
       <c r="J636" s="10"/>
@@ -21626,9 +21503,7 @@
         <v>1341</v>
       </c>
       <c r="F662" s="10"/>
-      <c r="G662" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G662" s="10"/>
       <c r="H662" s="10"/>
       <c r="I662" s="10"/>
       <c r="J662" s="10"/>
@@ -21653,13 +21528,9 @@
         <v>1343</v>
       </c>
       <c r="F663" s="10"/>
-      <c r="G663" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G663" s="10"/>
       <c r="H663" s="10"/>
-      <c r="I663" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="I663" s="10"/>
       <c r="J663" s="10"/>
       <c r="K663" s="10"/>
       <c r="L663" s="10"/>
@@ -21682,13 +21553,9 @@
         <v>1343</v>
       </c>
       <c r="F664" s="10"/>
-      <c r="G664" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G664" s="10"/>
       <c r="H664" s="10"/>
-      <c r="I664" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="I664" s="10"/>
       <c r="J664" s="10"/>
       <c r="K664" s="10"/>
       <c r="L664" s="10"/>
@@ -21711,13 +21578,9 @@
         <v>21</v>
       </c>
       <c r="F665" s="10"/>
-      <c r="G665" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G665" s="10"/>
       <c r="H665" s="10"/>
-      <c r="I665" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="I665" s="10"/>
       <c r="J665" s="10"/>
       <c r="K665" s="10"/>
       <c r="L665" s="10"/>
@@ -21840,9 +21703,7 @@
         <v>1354</v>
       </c>
       <c r="F670" s="10"/>
-      <c r="G670" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G670" s="10"/>
       <c r="H670" s="10"/>
       <c r="I670" s="10"/>
       <c r="J670" s="10"/>
@@ -21918,9 +21779,7 @@
       </c>
       <c r="F673" s="10"/>
       <c r="G673" s="10"/>
-      <c r="H673" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="H673" s="10"/>
       <c r="I673" s="10"/>
       <c r="J673" s="10"/>
       <c r="K673" s="10"/>
@@ -21944,9 +21803,7 @@
         <v>1363</v>
       </c>
       <c r="F674" s="10"/>
-      <c r="G674" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G674" s="10"/>
       <c r="H674" s="10"/>
       <c r="I674" s="10"/>
       <c r="J674" s="10"/>
@@ -21996,12 +21853,8 @@
         <v>21</v>
       </c>
       <c r="F676" s="10"/>
-      <c r="G676" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H676" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G676" s="10"/>
+      <c r="H676" s="10"/>
       <c r="I676" s="10"/>
       <c r="J676" s="10"/>
       <c r="K676" s="10"/>
@@ -22025,7 +21878,7 @@
         <v>1367</v>
       </c>
       <c r="F677" s="10"/>
-      <c r="G677" s="13"/>
+      <c r="G677" s="10"/>
       <c r="H677" s="10"/>
       <c r="I677" s="10"/>
       <c r="J677" s="10"/>
@@ -22050,7 +21903,7 @@
         <v>1367</v>
       </c>
       <c r="F678" s="10"/>
-      <c r="G678" s="13"/>
+      <c r="G678" s="10"/>
       <c r="H678" s="10"/>
       <c r="I678" s="10"/>
       <c r="J678" s="10"/>
@@ -22125,12 +21978,8 @@
         <v>1374</v>
       </c>
       <c r="F681" s="10"/>
-      <c r="G681" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H681" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G681" s="10"/>
+      <c r="H681" s="10"/>
       <c r="I681" s="10"/>
       <c r="J681" s="10"/>
       <c r="K681" s="10"/>
@@ -22533,7 +22382,9 @@
       <c r="H697" s="10"/>
       <c r="I697" s="10"/>
       <c r="J697" s="10"/>
-      <c r="K697" s="10"/>
+      <c r="K697" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="L697" s="10"/>
       <c r="M697" s="10"/>
     </row>
@@ -22705,7 +22556,9 @@
       </c>
       <c r="F704" s="10"/>
       <c r="G704" s="10"/>
-      <c r="H704" s="10"/>
+      <c r="H704" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="I704" s="10"/>
       <c r="J704" s="10"/>
       <c r="K704" s="10"/>
@@ -22779,9 +22632,7 @@
         <v>1429</v>
       </c>
       <c r="F707" s="10"/>
-      <c r="G707" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G707" s="10"/>
       <c r="H707" s="10"/>
       <c r="I707" s="10"/>
       <c r="J707" s="10"/>
@@ -22856,9 +22707,7 @@
         <v>1435</v>
       </c>
       <c r="F710" s="10"/>
-      <c r="G710" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G710" s="10"/>
       <c r="H710" s="10"/>
       <c r="I710" s="10"/>
       <c r="J710" s="10"/>
@@ -22933,12 +22782,8 @@
         <v>1441</v>
       </c>
       <c r="F713" s="10"/>
-      <c r="G713" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H713" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="G713" s="10"/>
+      <c r="H713" s="10"/>
       <c r="I713" s="10"/>
       <c r="J713" s="10"/>
       <c r="K713" s="10"/>
@@ -22974,7 +22819,6 @@
       <c r="H715" s="14"/>
     </row>
     <row r="716" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F716" s="10"/>
       <c r="H716" s="14"/>
     </row>
     <row r="717" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -23831,12 +23675,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>